<commit_message>
Modified exel file, tried some things
</commit_message>
<xml_diff>
--- a/test results/Human_Simple_Sample_Results.xlsx
+++ b/test results/Human_Simple_Sample_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarsan\Desktop\4740\test results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abarsan\Desktop\4740 P2\test results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Human_Simple_Sample_Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>q1</t>
   </si>
@@ -148,13 +148,37 @@
   </si>
   <si>
     <t>Context (L):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">std dev = </t>
+  </si>
+  <si>
+    <t>99% confidence interval:</t>
+  </si>
+  <si>
+    <t>0.47157 ≤ x ≤ 0.57843</t>
+  </si>
+  <si>
+    <t>95% confidence interval:</t>
+  </si>
+  <si>
+    <t>0.48491 ≤ x ≤ 0.56509</t>
+  </si>
+  <si>
+    <t>90% confidence interval:</t>
+  </si>
+  <si>
+    <t>0.49155 ≤ x ≤ 0.55845</t>
+  </si>
+  <si>
+    <t>using: http://www.danielsoper.com/statcalc3/calc.aspx?id=96</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,8 +320,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,6 +516,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -638,12 +683,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1047,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R26" sqref="R26"/>
+    <sheetView tabSelected="1" topLeftCell="J10" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1885,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1101</v>
       </c>
@@ -1884,7 +1935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>434</v>
       </c>
@@ -1934,7 +1985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>433</v>
       </c>
@@ -1987,7 +2038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>888</v>
       </c>
@@ -2040,7 +2091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>627</v>
       </c>
@@ -2081,7 +2132,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>201</v>
       </c>
@@ -2121,8 +2172,15 @@
       <c r="M22">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q22">
+        <f>STDEV(M2:M53)</f>
+        <v>0.14399754899874886</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>295</v>
       </c>
@@ -2163,7 +2221,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>198</v>
       </c>
@@ -2203,8 +2261,17 @@
       <c r="M24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>598</v>
       </c>
@@ -2244,8 +2311,14 @@
       <c r="M25">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>608</v>
       </c>
@@ -2285,8 +2358,14 @@
       <c r="M26">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>263</v>
       </c>
@@ -2327,7 +2406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>591</v>
       </c>
@@ -2368,7 +2447,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>515</v>
       </c>
@@ -2409,7 +2488,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>252</v>
       </c>
@@ -2450,7 +2529,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>434</v>
       </c>
@@ -2491,7 +2570,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>386</v>
       </c>

</xml_diff>